<commit_message>
Adding data by county of June 4th
</commit_message>
<xml_diff>
--- a/data-raw/bitácora_ssa.xlsx
+++ b/data-raw/bitácora_ssa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-nacional/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yadi/Documents/GitHub/covid19-mx-data/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9182FA99-23E5-0042-9C58-732E39332586}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F54EBB-D2CE-814B-8D4F-168140874327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38360" yWindow="4100" windowWidth="28800" windowHeight="17540" activeTab="6" xr2:uid="{EA61CC18-B893-42EC-B0EF-B2C064690A7F}"/>
+    <workbookView xWindow="10200" yWindow="3700" windowWidth="15400" windowHeight="12300" activeTab="5" xr2:uid="{EA61CC18-B893-42EC-B0EF-B2C064690A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -547,7 +547,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1003,7 +1003,7 @@
         <v>6581</v>
       </c>
       <c r="J3" s="11">
-        <f t="shared" ref="J3:J35" si="0">(I3/B3)</f>
+        <f t="shared" ref="J3:J34" si="0">(I3/B3)</f>
         <v>0.39284861509073543</v>
       </c>
       <c r="K3" s="6"/>
@@ -6528,8 +6528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCEFAF23-6504-B540-A827-4BCE378F0E12}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6544,7 +6544,9 @@
       <c r="C1" s="22">
         <v>43978</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="22">
+        <v>43986</v>
+      </c>
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
@@ -6564,6 +6566,9 @@
       <c r="C2" s="27">
         <v>61368</v>
       </c>
+      <c r="D2">
+        <v>74829</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
@@ -6575,6 +6580,9 @@
       <c r="C3">
         <v>54975</v>
       </c>
+      <c r="D3">
+        <v>67914</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
@@ -6586,6 +6594,9 @@
       <c r="C4">
         <v>54975</v>
       </c>
+      <c r="D4">
+        <v>67914</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
@@ -6597,6 +6608,9 @@
       <c r="C5">
         <v>54975</v>
       </c>
+      <c r="D5">
+        <v>67914</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
@@ -6608,6 +6622,9 @@
       <c r="C6">
         <v>54975</v>
       </c>
+      <c r="D6">
+        <v>67914</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
@@ -6619,6 +6636,9 @@
       <c r="C7">
         <v>24175</v>
       </c>
+      <c r="D7">
+        <v>31690</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
@@ -6630,6 +6650,9 @@
       <c r="C8">
         <v>113639</v>
       </c>
+      <c r="D8">
+        <v>129929</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
@@ -6645,6 +6668,10 @@
       <c r="C10">
         <f>SUM(C2:C8)</f>
         <v>419082</v>
+      </c>
+      <c r="D10">
+        <f>SUM(D2:D8)</f>
+        <v>508104</v>
       </c>
     </row>
   </sheetData>
@@ -6656,7 +6683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D853C6-E82A-4F69-B736-BB3A2FD2C788}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>